<commit_message>
Added saving to Excel Sheet
</commit_message>
<xml_diff>
--- a/NestedBinary Data.xlsx
+++ b/NestedBinary Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/benjaminkhoury/Documents/GitHub/AstroResearch/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD97B6CA-1821-2843-941B-4AD6D21400F2}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F53F18B8-2F68-194C-82EC-90876EEC2CDC}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="16420" xr2:uid="{D9EB7902-EF24-F54C-A97A-534E0EA0FFE4}"/>
+    <workbookView xWindow="1520" yWindow="5500" windowWidth="28040" windowHeight="16420" xr2:uid="{D9EB7902-EF24-F54C-A97A-534E0EA0FFE4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -180,9 +180,6 @@
     <t>-19.893211237176313 to 0.06537909917792345</t>
   </si>
   <si>
-    <t>Using NestedBinary, m1=m2=8, a1=2, t=10, e1=0, m1=1</t>
-  </si>
-  <si>
     <t>0.00011247668621964515 to 0.09353111510330075</t>
   </si>
   <si>
@@ -604,6 +601,9 @@
   </si>
   <si>
     <t>-1.6953882188415667e-5 to 0.0005105169857792341</t>
+  </si>
+  <si>
+    <t>Using NestedBinary, m1=m2=8, a1=2, t=10, e1=0, m3=1</t>
   </si>
 </sst>
 </file>
@@ -821,6 +821,57 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -828,57 +879,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1197,8 +1197,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4FE1FEAB-4EB5-8F4F-814F-6696925DD1DB}">
   <dimension ref="A1:J62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D34" zoomScale="99" workbookViewId="0">
-      <selection activeCell="D62" sqref="D62"/>
+    <sheetView tabSelected="1" zoomScale="99" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1216,15 +1216,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1" s="11" t="s">
-        <v>49</v>
-      </c>
-      <c r="B1" s="11"/>
-      <c r="C1" s="11"/>
-      <c r="D1" s="11"/>
-      <c r="E1" s="11"/>
-      <c r="F1" s="11"/>
-      <c r="G1" s="11"/>
+      <c r="A1" s="28" t="s">
+        <v>190</v>
+      </c>
+      <c r="B1" s="28"/>
+      <c r="C1" s="28"/>
+      <c r="D1" s="28"/>
+      <c r="E1" s="28"/>
+      <c r="F1" s="28"/>
+      <c r="G1" s="28"/>
     </row>
     <row r="2" spans="1:10" s="2" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
@@ -1242,7 +1242,7 @@
       <c r="E2" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="F2" s="14" t="s">
+      <c r="F2" s="11" t="s">
         <v>7</v>
       </c>
       <c r="G2" s="8" t="s">
@@ -1254,15 +1254,15 @@
       <c r="I2" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="J2" s="13" t="s">
+      <c r="J2" s="10" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A3" s="17">
+      <c r="A3" s="25">
         <v>5</v>
       </c>
-      <c r="B3" s="18">
+      <c r="B3" s="22">
         <v>0</v>
       </c>
       <c r="C3" s="3">
@@ -1274,19 +1274,19 @@
       <c r="E3" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="F3" s="15"/>
-      <c r="G3" s="12"/>
-      <c r="H3" s="12">
+      <c r="F3" s="12"/>
+      <c r="G3" s="9"/>
+      <c r="H3" s="9">
         <v>9.4934883999999997E-2</v>
       </c>
-      <c r="I3" s="12" t="s">
+      <c r="I3" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="J3" s="26"/>
+      <c r="J3" s="19"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A4" s="9"/>
-      <c r="B4" s="19"/>
+      <c r="A4" s="26"/>
+      <c r="B4" s="23"/>
       <c r="C4" s="3">
         <v>0.1</v>
       </c>
@@ -1296,18 +1296,18 @@
       <c r="E4" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="F4" s="16"/>
+      <c r="F4" s="13"/>
       <c r="H4" s="7">
         <v>9.8910234999999999E-2</v>
       </c>
       <c r="I4" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="J4" s="24"/>
+      <c r="J4" s="17"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A5" s="9"/>
-      <c r="B5" s="19"/>
+      <c r="A5" s="26"/>
+      <c r="B5" s="23"/>
       <c r="C5" s="3">
         <v>0.01</v>
       </c>
@@ -1317,18 +1317,18 @@
       <c r="E5" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="F5" s="16"/>
+      <c r="F5" s="13"/>
       <c r="H5" s="7">
         <v>0.50495217699999995</v>
       </c>
       <c r="I5" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="J5" s="25"/>
+      <c r="J5" s="18"/>
     </row>
     <row r="6" spans="1:10" s="2" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="9"/>
-      <c r="B6" s="20"/>
+      <c r="A6" s="26"/>
+      <c r="B6" s="24"/>
       <c r="C6" s="6">
         <v>1E-3</v>
       </c>
@@ -1338,7 +1338,7 @@
       <c r="E6" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="F6" s="14"/>
+      <c r="F6" s="11"/>
       <c r="G6" s="8"/>
       <c r="H6" s="8">
         <v>4.5092421140000001</v>
@@ -1346,11 +1346,11 @@
       <c r="I6" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="J6" s="27"/>
+      <c r="J6" s="20"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A7" s="9"/>
-      <c r="B7" s="18">
+      <c r="A7" s="26"/>
+      <c r="B7" s="22">
         <v>0.25</v>
       </c>
       <c r="C7" s="7">
@@ -1362,18 +1362,18 @@
       <c r="E7" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="F7" s="16"/>
+      <c r="F7" s="13"/>
       <c r="H7" s="7">
         <v>0.19593264499999999</v>
       </c>
       <c r="I7" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="J7" s="26"/>
+      <c r="J7" s="19"/>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A8" s="9"/>
-      <c r="B8" s="19"/>
+      <c r="A8" s="26"/>
+      <c r="B8" s="23"/>
       <c r="C8" s="7">
         <v>0.01</v>
       </c>
@@ -1383,18 +1383,18 @@
       <c r="E8" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="F8" s="16"/>
+      <c r="F8" s="13"/>
       <c r="H8" s="7">
         <v>0.45818740299999999</v>
       </c>
       <c r="I8" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="J8" s="24"/>
+      <c r="J8" s="17"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A9" s="9"/>
-      <c r="B9" s="19"/>
+      <c r="A9" s="26"/>
+      <c r="B9" s="23"/>
       <c r="C9" s="3">
         <v>1E-3</v>
       </c>
@@ -1410,11 +1410,11 @@
       <c r="I9" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="J9" s="24"/>
+      <c r="J9" s="17"/>
     </row>
     <row r="10" spans="1:10" s="2" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="9"/>
-      <c r="B10" s="20"/>
+      <c r="A10" s="26"/>
+      <c r="B10" s="24"/>
       <c r="C10" s="6">
         <v>1E-4</v>
       </c>
@@ -1424,7 +1424,7 @@
       <c r="E10" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="F10" s="14"/>
+      <c r="F10" s="11"/>
       <c r="G10" s="8"/>
       <c r="H10" s="8">
         <v>242.73521456099999</v>
@@ -1432,11 +1432,11 @@
       <c r="I10" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="J10" s="27"/>
+      <c r="J10" s="20"/>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A11" s="9"/>
-      <c r="B11" s="18">
+      <c r="A11" s="26"/>
+      <c r="B11" s="22">
         <v>0.5</v>
       </c>
       <c r="C11" s="7">
@@ -1448,18 +1448,18 @@
       <c r="E11" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="F11" s="16"/>
+      <c r="F11" s="13"/>
       <c r="H11" s="7">
         <v>0.127535017</v>
       </c>
       <c r="I11" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="J11" s="26"/>
+      <c r="J11" s="19"/>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A12" s="9"/>
-      <c r="B12" s="19"/>
+      <c r="A12" s="26"/>
+      <c r="B12" s="23"/>
       <c r="C12" s="7">
         <v>0.01</v>
       </c>
@@ -1469,18 +1469,18 @@
       <c r="E12" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="F12" s="16"/>
+      <c r="F12" s="13"/>
       <c r="H12" s="7">
         <v>0.17747136899999999</v>
       </c>
       <c r="I12" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="J12" s="24"/>
+      <c r="J12" s="17"/>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A13" s="9"/>
-      <c r="B13" s="19"/>
+      <c r="A13" s="26"/>
+      <c r="B13" s="23"/>
       <c r="C13" s="7">
         <v>1E-3</v>
       </c>
@@ -1490,18 +1490,18 @@
       <c r="E13" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="F13" s="16"/>
+      <c r="F13" s="13"/>
       <c r="H13" s="7">
         <v>1.1393391530000001</v>
       </c>
       <c r="I13" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="J13" s="24"/>
+      <c r="J13" s="17"/>
     </row>
     <row r="14" spans="1:10" s="2" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="9"/>
-      <c r="B14" s="20"/>
+      <c r="A14" s="26"/>
+      <c r="B14" s="24"/>
       <c r="C14" s="6">
         <v>1E-4</v>
       </c>
@@ -1511,7 +1511,7 @@
       <c r="E14" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="F14" s="14"/>
+      <c r="F14" s="11"/>
       <c r="G14" s="8"/>
       <c r="H14" s="8">
         <v>4.4069475899999997</v>
@@ -1519,1068 +1519,1070 @@
       <c r="I14" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="J14" s="28"/>
+      <c r="J14" s="21"/>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A15" s="9"/>
-      <c r="B15" s="18">
+      <c r="A15" s="26"/>
+      <c r="B15" s="22">
         <v>0.75</v>
       </c>
       <c r="C15" s="7">
         <v>0.1</v>
       </c>
-      <c r="D15" s="21" t="s">
+      <c r="D15" s="14" t="s">
         <v>48</v>
       </c>
-      <c r="E15" s="12" t="s">
+      <c r="E15" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="F15" s="15"/>
-      <c r="G15" s="12"/>
-      <c r="H15" s="12">
+      <c r="F15" s="12"/>
+      <c r="G15" s="9"/>
+      <c r="H15" s="9">
         <v>8.5699282000000002E-2</v>
       </c>
-      <c r="I15" s="12" t="s">
+      <c r="I15" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="J15" s="24"/>
+      <c r="J15" s="17"/>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A16" s="9"/>
-      <c r="B16" s="19"/>
+      <c r="A16" s="26"/>
+      <c r="B16" s="23"/>
       <c r="C16" s="7">
         <v>0.01</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E16" s="7" t="s">
-        <v>51</v>
-      </c>
-      <c r="F16" s="16"/>
+        <v>50</v>
+      </c>
+      <c r="F16" s="13"/>
       <c r="H16" s="7">
         <v>0.266577697</v>
       </c>
       <c r="I16" s="7" t="s">
-        <v>50</v>
-      </c>
-      <c r="J16" s="24"/>
+        <v>49</v>
+      </c>
+      <c r="J16" s="17"/>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A17" s="9"/>
-      <c r="B17" s="19"/>
+      <c r="A17" s="26"/>
+      <c r="B17" s="23"/>
       <c r="C17" s="7">
         <v>1E-3</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E17" s="7" t="s">
-        <v>54</v>
-      </c>
-      <c r="F17" s="16"/>
+        <v>53</v>
+      </c>
+      <c r="F17" s="13"/>
       <c r="H17" s="7">
         <v>0.60971342399999995</v>
       </c>
       <c r="I17" s="7" t="s">
-        <v>53</v>
-      </c>
-      <c r="J17" s="24"/>
+        <v>52</v>
+      </c>
+      <c r="J17" s="17"/>
     </row>
     <row r="18" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="9"/>
-      <c r="B18" s="20"/>
+      <c r="A18" s="26"/>
+      <c r="B18" s="24"/>
       <c r="C18" s="6">
         <v>1E-4</v>
       </c>
       <c r="D18" s="6" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E18" s="8" t="s">
-        <v>57</v>
-      </c>
-      <c r="F18" s="14"/>
+        <v>56</v>
+      </c>
+      <c r="F18" s="11"/>
       <c r="G18" s="8"/>
       <c r="H18" s="8">
         <v>3.441144091</v>
       </c>
       <c r="I18" s="8" t="s">
-        <v>56</v>
-      </c>
-      <c r="J18" s="24"/>
+        <v>55</v>
+      </c>
+      <c r="J18" s="17"/>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A19" s="9"/>
-      <c r="B19" s="19">
+      <c r="A19" s="26"/>
+      <c r="B19" s="23">
         <v>0.99</v>
       </c>
       <c r="C19" s="7">
         <v>0.1</v>
       </c>
       <c r="D19" s="5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E19" s="7" t="s">
-        <v>60</v>
-      </c>
-      <c r="F19" s="16"/>
+        <v>59</v>
+      </c>
+      <c r="F19" s="13"/>
       <c r="H19" s="7">
         <v>7.3081613000000004E-2</v>
       </c>
       <c r="I19" s="7" t="s">
-        <v>59</v>
-      </c>
-      <c r="J19" s="24"/>
+        <v>58</v>
+      </c>
+      <c r="J19" s="17"/>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A20" s="9"/>
-      <c r="B20" s="19"/>
+      <c r="A20" s="26"/>
+      <c r="B20" s="23"/>
       <c r="C20" s="7">
         <v>0.01</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E20" s="7" t="s">
-        <v>63</v>
-      </c>
-      <c r="F20" s="16"/>
+        <v>62</v>
+      </c>
+      <c r="F20" s="13"/>
       <c r="H20" s="7">
         <v>0.98725858600000005</v>
       </c>
       <c r="I20" s="7" t="s">
-        <v>62</v>
-      </c>
-      <c r="J20" s="24"/>
+        <v>61</v>
+      </c>
+      <c r="J20" s="17"/>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A21" s="9"/>
-      <c r="B21" s="19"/>
+      <c r="A21" s="26"/>
+      <c r="B21" s="23"/>
       <c r="C21" s="7">
         <v>1E-3</v>
       </c>
       <c r="D21" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="E21" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="E21" s="7" t="s">
-        <v>66</v>
-      </c>
-      <c r="F21" s="16"/>
+      <c r="F21" s="13"/>
       <c r="H21" s="7">
         <v>1.5038266810000001</v>
       </c>
       <c r="I21" s="7" t="s">
-        <v>67</v>
-      </c>
-      <c r="J21" s="24"/>
+        <v>66</v>
+      </c>
+      <c r="J21" s="17"/>
     </row>
     <row r="22" spans="1:10" s="2" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="10"/>
-      <c r="B22" s="20"/>
+      <c r="A22" s="27"/>
+      <c r="B22" s="24"/>
       <c r="C22" s="6">
         <v>1E-4</v>
       </c>
       <c r="D22" s="6" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E22" s="8" t="s">
-        <v>69</v>
-      </c>
-      <c r="F22" s="14"/>
+        <v>68</v>
+      </c>
+      <c r="F22" s="11"/>
       <c r="G22" s="8"/>
       <c r="H22" s="8">
         <v>10.541763982000001</v>
       </c>
       <c r="I22" s="8" t="s">
-        <v>68</v>
-      </c>
-      <c r="J22" s="24"/>
+        <v>67</v>
+      </c>
+      <c r="J22" s="17"/>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A23" s="17">
+      <c r="A23" s="25">
         <v>10</v>
       </c>
-      <c r="B23" s="18">
+      <c r="B23" s="22">
         <v>0</v>
       </c>
       <c r="C23" s="7">
         <v>0.1</v>
       </c>
       <c r="D23" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="E23" s="7" t="s">
         <v>71</v>
       </c>
-      <c r="E23" s="7" t="s">
+      <c r="F23" s="12"/>
+      <c r="G23" s="9"/>
+      <c r="H23" s="9">
+        <v>0.170551223</v>
+      </c>
+      <c r="I23" s="9" t="s">
         <v>72</v>
       </c>
-      <c r="F23" s="15"/>
-      <c r="G23" s="12"/>
-      <c r="H23" s="12">
-        <v>0.170551223</v>
-      </c>
-      <c r="I23" s="12" t="s">
-        <v>73</v>
-      </c>
-      <c r="J23" s="24"/>
+      <c r="J23" s="17"/>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A24" s="9"/>
-      <c r="B24" s="19"/>
+      <c r="A24" s="26"/>
+      <c r="B24" s="23"/>
       <c r="C24" s="7">
         <v>0.01</v>
       </c>
       <c r="D24" s="5" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E24" s="7" t="s">
-        <v>74</v>
-      </c>
-      <c r="F24" s="16"/>
+        <v>73</v>
+      </c>
+      <c r="F24" s="13"/>
       <c r="H24" s="7">
         <v>0.269969862</v>
       </c>
       <c r="I24" s="7" t="s">
-        <v>76</v>
-      </c>
-      <c r="J24" s="24"/>
+        <v>75</v>
+      </c>
+      <c r="J24" s="17"/>
     </row>
     <row r="25" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="9"/>
-      <c r="B25" s="19"/>
+      <c r="A25" s="26"/>
+      <c r="B25" s="23"/>
       <c r="C25" s="7">
         <v>1E-3</v>
       </c>
       <c r="D25" s="5" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E25" s="7" t="s">
-        <v>78</v>
-      </c>
-      <c r="F25" s="16"/>
+        <v>77</v>
+      </c>
+      <c r="F25" s="13"/>
       <c r="H25" s="7">
         <v>1.6534984429999999</v>
       </c>
       <c r="I25" s="7" t="s">
-        <v>77</v>
-      </c>
-      <c r="J25" s="27"/>
+        <v>76</v>
+      </c>
+      <c r="J25" s="20"/>
     </row>
     <row r="26" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="9"/>
-      <c r="B26" s="20"/>
+      <c r="A26" s="26"/>
+      <c r="B26" s="24"/>
       <c r="C26" s="6">
         <v>1E-4</v>
       </c>
       <c r="D26" s="6" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E26" s="8" t="s">
-        <v>81</v>
-      </c>
-      <c r="F26" s="14"/>
+        <v>80</v>
+      </c>
+      <c r="F26" s="11"/>
       <c r="G26" s="8"/>
       <c r="H26" s="8">
         <v>19.788413944999999</v>
       </c>
       <c r="I26" s="8" t="s">
-        <v>80</v>
-      </c>
-      <c r="J26" s="27"/>
+        <v>79</v>
+      </c>
+      <c r="J26" s="20"/>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A27" s="9"/>
-      <c r="B27" s="18">
+      <c r="A27" s="26"/>
+      <c r="B27" s="22">
         <v>0.25</v>
       </c>
       <c r="C27" s="7">
         <v>0.1</v>
       </c>
       <c r="D27" s="5" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E27" s="7" t="s">
-        <v>84</v>
-      </c>
-      <c r="F27" s="16"/>
+        <v>83</v>
+      </c>
+      <c r="F27" s="13"/>
       <c r="H27" s="7">
         <v>9.5702733999999998E-2</v>
       </c>
       <c r="I27" s="7" t="s">
-        <v>83</v>
-      </c>
-      <c r="J27" s="24"/>
+        <v>82</v>
+      </c>
+      <c r="J27" s="17"/>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A28" s="9"/>
-      <c r="B28" s="19"/>
+      <c r="A28" s="26"/>
+      <c r="B28" s="23"/>
       <c r="C28" s="7">
         <v>0.01</v>
       </c>
       <c r="D28" s="5" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E28" s="7" t="s">
-        <v>88</v>
-      </c>
-      <c r="F28" s="16"/>
+        <v>87</v>
+      </c>
+      <c r="F28" s="13"/>
       <c r="H28" s="7">
         <v>0.18819638799999999</v>
       </c>
       <c r="I28" s="7" t="s">
-        <v>87</v>
-      </c>
-      <c r="J28" s="24"/>
+        <v>86</v>
+      </c>
+      <c r="J28" s="17"/>
     </row>
     <row r="29" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="9"/>
-      <c r="B29" s="19"/>
+      <c r="A29" s="26"/>
+      <c r="B29" s="23"/>
       <c r="C29" s="7">
         <v>1E-3</v>
       </c>
       <c r="D29" s="5" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E29" s="7" t="s">
-        <v>90</v>
-      </c>
-      <c r="F29" s="16"/>
+        <v>89</v>
+      </c>
+      <c r="F29" s="13"/>
       <c r="H29" s="7">
         <v>3.1612408429999999</v>
       </c>
       <c r="I29" s="7" t="s">
-        <v>89</v>
-      </c>
-      <c r="J29" s="27"/>
+        <v>88</v>
+      </c>
+      <c r="J29" s="20"/>
     </row>
     <row r="30" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="9"/>
-      <c r="B30" s="20"/>
+      <c r="A30" s="26"/>
+      <c r="B30" s="24"/>
       <c r="C30" s="6">
         <v>1E-4</v>
       </c>
       <c r="D30" s="6" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E30" s="8" t="s">
-        <v>93</v>
-      </c>
-      <c r="F30" s="14"/>
+        <v>92</v>
+      </c>
+      <c r="F30" s="11"/>
       <c r="G30" s="8"/>
       <c r="H30" s="8">
         <v>26.417612762000001</v>
       </c>
       <c r="I30" s="8" t="s">
-        <v>92</v>
-      </c>
-      <c r="J30" s="27"/>
+        <v>91</v>
+      </c>
+      <c r="J30" s="20"/>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A31" s="9"/>
-      <c r="B31" s="18">
+      <c r="A31" s="26"/>
+      <c r="B31" s="22">
         <v>0.5</v>
       </c>
       <c r="C31" s="7">
         <v>0.1</v>
       </c>
       <c r="D31" s="5" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E31" s="7" t="s">
-        <v>96</v>
-      </c>
-      <c r="F31" s="16"/>
+        <v>95</v>
+      </c>
+      <c r="F31" s="13"/>
       <c r="H31" s="7">
         <v>6.4536439000000001E-2</v>
       </c>
       <c r="I31" s="7" t="s">
-        <v>95</v>
-      </c>
-      <c r="J31" s="24"/>
+        <v>94</v>
+      </c>
+      <c r="J31" s="17"/>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A32" s="9"/>
-      <c r="B32" s="19"/>
+      <c r="A32" s="26"/>
+      <c r="B32" s="23"/>
       <c r="C32" s="7">
         <v>0.01</v>
       </c>
       <c r="D32" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="E32" s="7" t="s">
         <v>98</v>
       </c>
-      <c r="E32" s="7" t="s">
-        <v>99</v>
-      </c>
-      <c r="F32" s="16"/>
+      <c r="F32" s="13"/>
       <c r="H32" s="7">
         <v>0.30375160299999998</v>
       </c>
       <c r="I32" s="7" t="s">
-        <v>100</v>
-      </c>
-      <c r="J32" s="24"/>
+        <v>99</v>
+      </c>
+      <c r="J32" s="17"/>
     </row>
     <row r="33" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="9"/>
-      <c r="B33" s="19"/>
+      <c r="A33" s="26"/>
+      <c r="B33" s="23"/>
       <c r="C33" s="7">
         <v>1E-3</v>
       </c>
       <c r="D33" s="5" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E33" s="7" t="s">
-        <v>102</v>
-      </c>
-      <c r="F33" s="16"/>
+        <v>101</v>
+      </c>
+      <c r="F33" s="13"/>
       <c r="H33" s="7">
         <v>0.51101821300000005</v>
       </c>
       <c r="I33" s="7" t="s">
-        <v>101</v>
-      </c>
-      <c r="J33" s="28"/>
+        <v>100</v>
+      </c>
+      <c r="J33" s="21"/>
     </row>
     <row r="34" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="9"/>
-      <c r="B34" s="20"/>
+      <c r="A34" s="26"/>
+      <c r="B34" s="24"/>
       <c r="C34" s="6">
         <v>1E-4</v>
       </c>
       <c r="D34" s="6" t="s">
+        <v>104</v>
+      </c>
+      <c r="E34" s="8" t="s">
         <v>105</v>
       </c>
-      <c r="E34" s="8" t="s">
-        <v>106</v>
-      </c>
-      <c r="F34" s="14"/>
+      <c r="F34" s="11"/>
       <c r="G34" s="8"/>
       <c r="H34" s="8">
         <v>3.9264369000000001</v>
       </c>
       <c r="I34" s="8" t="s">
-        <v>104</v>
-      </c>
-      <c r="J34" s="28"/>
+        <v>103</v>
+      </c>
+      <c r="J34" s="21"/>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A35" s="9"/>
-      <c r="B35" s="18">
+      <c r="A35" s="26"/>
+      <c r="B35" s="22">
         <v>0.75</v>
       </c>
       <c r="C35" s="7">
         <v>0.1</v>
       </c>
-      <c r="D35" s="21" t="s">
-        <v>109</v>
-      </c>
-      <c r="E35" s="12" t="s">
+      <c r="D35" s="14" t="s">
         <v>108</v>
       </c>
-      <c r="F35" s="15"/>
-      <c r="G35" s="12"/>
-      <c r="H35" s="12">
+      <c r="E35" s="9" t="s">
+        <v>107</v>
+      </c>
+      <c r="F35" s="12"/>
+      <c r="G35" s="9"/>
+      <c r="H35" s="9">
         <v>6.3409884E-2</v>
       </c>
-      <c r="I35" s="12" t="s">
-        <v>107</v>
-      </c>
-      <c r="J35" s="24"/>
+      <c r="I35" s="9" t="s">
+        <v>106</v>
+      </c>
+      <c r="J35" s="17"/>
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A36" s="9"/>
-      <c r="B36" s="19"/>
+      <c r="A36" s="26"/>
+      <c r="B36" s="23"/>
       <c r="C36" s="7">
         <v>0.01</v>
       </c>
       <c r="D36" s="5" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E36" s="7" t="s">
-        <v>111</v>
-      </c>
-      <c r="F36" s="16"/>
+        <v>110</v>
+      </c>
+      <c r="F36" s="13"/>
       <c r="H36" s="7">
         <v>9.9729718999999994E-2</v>
       </c>
       <c r="I36" s="7" t="s">
-        <v>110</v>
-      </c>
-      <c r="J36" s="24"/>
+        <v>109</v>
+      </c>
+      <c r="J36" s="17"/>
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A37" s="9"/>
-      <c r="B37" s="19"/>
+      <c r="A37" s="26"/>
+      <c r="B37" s="23"/>
       <c r="C37" s="7">
         <v>1E-3</v>
       </c>
       <c r="D37" s="5" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="E37" s="7" t="s">
-        <v>113</v>
-      </c>
-      <c r="F37" s="16"/>
+        <v>112</v>
+      </c>
+      <c r="F37" s="13"/>
       <c r="H37" s="7">
         <v>0.750410307</v>
       </c>
       <c r="I37" s="7" t="s">
-        <v>115</v>
-      </c>
-      <c r="J37" s="24"/>
+        <v>114</v>
+      </c>
+      <c r="J37" s="17"/>
     </row>
     <row r="38" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="9"/>
-      <c r="B38" s="20"/>
+      <c r="A38" s="26"/>
+      <c r="B38" s="24"/>
       <c r="C38" s="6">
         <v>1E-4</v>
       </c>
       <c r="D38" s="6" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E38" s="8" t="s">
-        <v>117</v>
-      </c>
-      <c r="F38" s="14"/>
+        <v>116</v>
+      </c>
+      <c r="F38" s="11"/>
       <c r="G38" s="8"/>
       <c r="H38" s="8">
         <v>4.5653128709999997</v>
       </c>
       <c r="I38" s="8" t="s">
-        <v>116</v>
-      </c>
-      <c r="J38" s="24"/>
+        <v>115</v>
+      </c>
+      <c r="J38" s="17"/>
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A39" s="9"/>
-      <c r="B39" s="19">
+      <c r="A39" s="26"/>
+      <c r="B39" s="23">
         <v>0.99</v>
       </c>
       <c r="C39" s="7">
         <v>0.1</v>
       </c>
       <c r="D39" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="E39" s="7" t="s">
         <v>119</v>
       </c>
-      <c r="E39" s="7" t="s">
-        <v>120</v>
-      </c>
-      <c r="F39" s="16"/>
+      <c r="F39" s="13"/>
       <c r="H39" s="7">
         <v>6.3844456999999993E-2</v>
       </c>
       <c r="I39" s="7" t="s">
-        <v>121</v>
-      </c>
-      <c r="J39" s="24"/>
+        <v>120</v>
+      </c>
+      <c r="J39" s="17"/>
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A40" s="9"/>
-      <c r="B40" s="19"/>
+      <c r="A40" s="26"/>
+      <c r="B40" s="23"/>
       <c r="C40" s="7">
         <v>0.01</v>
       </c>
       <c r="D40" s="5" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="E40" s="7" t="s">
-        <v>123</v>
-      </c>
-      <c r="F40" s="16"/>
+        <v>122</v>
+      </c>
+      <c r="F40" s="13"/>
       <c r="H40" s="7">
         <v>0.190366655</v>
       </c>
       <c r="I40" s="7" t="s">
-        <v>122</v>
-      </c>
-      <c r="J40" s="24"/>
+        <v>121</v>
+      </c>
+      <c r="J40" s="17"/>
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A41" s="9"/>
-      <c r="B41" s="19"/>
+      <c r="A41" s="26"/>
+      <c r="B41" s="23"/>
       <c r="C41" s="7">
         <v>1E-3</v>
       </c>
       <c r="D41" s="5" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="E41" s="7" t="s">
-        <v>126</v>
-      </c>
-      <c r="F41" s="16"/>
+        <v>125</v>
+      </c>
+      <c r="F41" s="13"/>
       <c r="H41" s="7">
         <v>0.33415682400000002</v>
       </c>
       <c r="I41" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="J41" s="24"/>
+        <v>124</v>
+      </c>
+      <c r="J41" s="17"/>
     </row>
     <row r="42" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="10"/>
-      <c r="B42" s="20"/>
+      <c r="A42" s="27"/>
+      <c r="B42" s="24"/>
       <c r="C42" s="6">
         <v>1E-4</v>
       </c>
       <c r="D42" s="6" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="E42" s="8" t="s">
-        <v>129</v>
-      </c>
-      <c r="F42" s="14"/>
+        <v>128</v>
+      </c>
+      <c r="F42" s="11"/>
       <c r="G42" s="8"/>
       <c r="H42" s="8">
         <v>2.856699205</v>
       </c>
       <c r="I42" s="8" t="s">
-        <v>128</v>
-      </c>
-      <c r="J42" s="24"/>
+        <v>127</v>
+      </c>
+      <c r="J42" s="17"/>
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A43" s="17">
+      <c r="A43" s="25">
         <v>20</v>
       </c>
-      <c r="B43" s="18">
+      <c r="B43" s="22">
         <v>0</v>
       </c>
-      <c r="C43" s="22">
+      <c r="C43" s="15">
         <v>0.1</v>
       </c>
       <c r="D43" s="5" t="s">
+        <v>132</v>
+      </c>
+      <c r="E43" s="7" t="s">
+        <v>131</v>
+      </c>
+      <c r="F43" s="12"/>
+      <c r="G43" s="9"/>
+      <c r="H43" s="9">
+        <v>0.29748500300000003</v>
+      </c>
+      <c r="I43" s="9" t="s">
+        <v>130</v>
+      </c>
+      <c r="J43" s="17"/>
+    </row>
+    <row r="44" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="26"/>
+      <c r="B44" s="23"/>
+      <c r="C44" s="15">
+        <v>0.01</v>
+      </c>
+      <c r="D44" s="5" t="s">
+        <v>134</v>
+      </c>
+      <c r="E44" s="7" t="s">
         <v>133</v>
       </c>
-      <c r="E43" s="7" t="s">
-        <v>132</v>
-      </c>
-      <c r="F43" s="15"/>
-      <c r="G43" s="12"/>
-      <c r="H43" s="12">
-        <v>0.29748500300000003</v>
-      </c>
-      <c r="I43" s="12" t="s">
-        <v>131</v>
-      </c>
-      <c r="J43" s="24"/>
-    </row>
-    <row r="44" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="9"/>
-      <c r="B44" s="19"/>
-      <c r="C44" s="22">
-        <v>0.01</v>
-      </c>
-      <c r="D44" s="5" t="s">
-        <v>135</v>
-      </c>
-      <c r="E44" s="7" t="s">
-        <v>134</v>
-      </c>
-      <c r="F44" s="16"/>
+      <c r="F44" s="13"/>
       <c r="H44" s="7">
         <v>0.20831961199999999</v>
       </c>
       <c r="I44" s="7" t="s">
-        <v>136</v>
-      </c>
-      <c r="J44" s="27"/>
+        <v>135</v>
+      </c>
+      <c r="J44" s="20"/>
     </row>
     <row r="45" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="9"/>
-      <c r="B45" s="19"/>
-      <c r="C45" s="22">
+      <c r="A45" s="26"/>
+      <c r="B45" s="23"/>
+      <c r="C45" s="15">
         <v>1E-3</v>
       </c>
       <c r="D45" s="5" t="s">
+        <v>137</v>
+      </c>
+      <c r="E45" s="7" t="s">
         <v>138</v>
       </c>
-      <c r="E45" s="7" t="s">
-        <v>139</v>
-      </c>
-      <c r="F45" s="16"/>
+      <c r="F45" s="13"/>
       <c r="H45" s="7">
         <v>0.93698309700000004</v>
       </c>
       <c r="I45" s="7" t="s">
-        <v>137</v>
-      </c>
-      <c r="J45" s="27"/>
+        <v>136</v>
+      </c>
+      <c r="J45" s="20"/>
     </row>
     <row r="46" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="9"/>
-      <c r="B46" s="20"/>
-      <c r="C46" s="23">
+      <c r="A46" s="26"/>
+      <c r="B46" s="24"/>
+      <c r="C46" s="16">
         <v>1E-4</v>
       </c>
       <c r="D46" s="6" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E46" s="8" t="s">
-        <v>141</v>
-      </c>
-      <c r="F46" s="14"/>
+        <v>140</v>
+      </c>
+      <c r="F46" s="11"/>
       <c r="G46" s="8"/>
       <c r="H46" s="8">
         <v>9.1635846490000006</v>
       </c>
       <c r="I46" s="8" t="s">
-        <v>140</v>
-      </c>
-      <c r="J46" s="27"/>
+        <v>139</v>
+      </c>
+      <c r="J46" s="20"/>
     </row>
     <row r="47" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A47" s="9"/>
-      <c r="B47" s="18">
+      <c r="A47" s="26"/>
+      <c r="B47" s="22">
         <v>0.25</v>
       </c>
-      <c r="C47" s="22">
+      <c r="C47" s="15">
         <v>0.1</v>
       </c>
       <c r="D47" s="5" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="E47" s="7" t="s">
-        <v>144</v>
-      </c>
-      <c r="F47" s="16"/>
+        <v>143</v>
+      </c>
+      <c r="F47" s="13"/>
       <c r="H47" s="7">
         <v>0.16110567200000001</v>
       </c>
       <c r="I47" s="7" t="s">
-        <v>143</v>
-      </c>
-      <c r="J47" s="24"/>
+        <v>142</v>
+      </c>
+      <c r="J47" s="17"/>
     </row>
     <row r="48" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A48" s="9"/>
-      <c r="B48" s="19"/>
-      <c r="C48" s="22">
+      <c r="A48" s="26"/>
+      <c r="B48" s="23"/>
+      <c r="C48" s="15">
         <v>0.01</v>
       </c>
       <c r="D48" s="5" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="E48" s="7" t="s">
-        <v>147</v>
-      </c>
-      <c r="F48" s="16"/>
+        <v>146</v>
+      </c>
+      <c r="F48" s="13"/>
       <c r="H48" s="7">
         <v>0.227109639</v>
       </c>
       <c r="I48" s="7" t="s">
-        <v>146</v>
-      </c>
-      <c r="J48" s="24"/>
+        <v>145</v>
+      </c>
+      <c r="J48" s="17"/>
     </row>
     <row r="49" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="9"/>
-      <c r="B49" s="19"/>
-      <c r="C49" s="22">
+      <c r="A49" s="26"/>
+      <c r="B49" s="23"/>
+      <c r="C49" s="15">
         <v>1E-3</v>
       </c>
       <c r="D49" s="5" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="E49" s="7" t="s">
-        <v>149</v>
-      </c>
-      <c r="F49" s="16"/>
+        <v>148</v>
+      </c>
+      <c r="F49" s="13"/>
       <c r="H49" s="7">
         <v>1.080497783</v>
       </c>
       <c r="I49" s="7" t="s">
-        <v>151</v>
-      </c>
-      <c r="J49" s="27"/>
+        <v>150</v>
+      </c>
+      <c r="J49" s="20"/>
     </row>
     <row r="50" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="9"/>
-      <c r="B50" s="20"/>
-      <c r="C50" s="23">
+      <c r="A50" s="26"/>
+      <c r="B50" s="24"/>
+      <c r="C50" s="16">
         <v>1E-4</v>
       </c>
       <c r="D50" s="6" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="E50" s="8" t="s">
-        <v>153</v>
-      </c>
-      <c r="F50" s="14"/>
+        <v>152</v>
+      </c>
+      <c r="F50" s="11"/>
       <c r="G50" s="8"/>
       <c r="H50" s="8">
         <v>10.648167883999999</v>
       </c>
       <c r="I50" s="8" t="s">
-        <v>152</v>
-      </c>
-      <c r="J50" s="27"/>
+        <v>151</v>
+      </c>
+      <c r="J50" s="20"/>
     </row>
     <row r="51" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A51" s="9"/>
-      <c r="B51" s="18">
+      <c r="A51" s="26"/>
+      <c r="B51" s="22">
         <v>0.5</v>
       </c>
-      <c r="C51" s="22">
+      <c r="C51" s="15">
         <v>0.1</v>
       </c>
       <c r="D51" s="5" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="E51" s="7" t="s">
-        <v>156</v>
-      </c>
-      <c r="F51" s="16"/>
+        <v>155</v>
+      </c>
+      <c r="F51" s="13"/>
       <c r="H51" s="7">
         <v>0.26135151299999998</v>
       </c>
       <c r="I51" s="7" t="s">
-        <v>155</v>
-      </c>
-      <c r="J51" s="24"/>
+        <v>154</v>
+      </c>
+      <c r="J51" s="17"/>
     </row>
     <row r="52" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A52" s="9"/>
-      <c r="B52" s="19"/>
-      <c r="C52" s="22">
+      <c r="A52" s="26"/>
+      <c r="B52" s="23"/>
+      <c r="C52" s="15">
         <v>0.01</v>
       </c>
       <c r="D52" s="5" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="E52" s="7" t="s">
-        <v>159</v>
-      </c>
-      <c r="F52" s="16"/>
+        <v>158</v>
+      </c>
+      <c r="F52" s="13"/>
       <c r="H52" s="7">
         <v>0.34195728800000003</v>
       </c>
       <c r="I52" s="7" t="s">
-        <v>158</v>
-      </c>
-      <c r="J52" s="24"/>
+        <v>157</v>
+      </c>
+      <c r="J52" s="17"/>
     </row>
     <row r="53" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="9"/>
-      <c r="B53" s="19"/>
-      <c r="C53" s="22">
+      <c r="A53" s="26"/>
+      <c r="B53" s="23"/>
+      <c r="C53" s="15">
         <v>1E-3</v>
       </c>
       <c r="D53" s="5" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="E53" s="7" t="s">
-        <v>162</v>
-      </c>
-      <c r="F53" s="16"/>
+        <v>161</v>
+      </c>
+      <c r="F53" s="13"/>
       <c r="H53" s="7">
         <v>1.346035034</v>
       </c>
       <c r="I53" s="7" t="s">
-        <v>161</v>
-      </c>
-      <c r="J53" s="27"/>
+        <v>160</v>
+      </c>
+      <c r="J53" s="20"/>
     </row>
     <row r="54" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="9"/>
-      <c r="B54" s="20"/>
-      <c r="C54" s="23">
+      <c r="A54" s="26"/>
+      <c r="B54" s="24"/>
+      <c r="C54" s="16">
         <v>1E-4</v>
       </c>
       <c r="D54" s="6" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="E54" s="8" t="s">
-        <v>165</v>
-      </c>
-      <c r="F54" s="14"/>
+        <v>164</v>
+      </c>
+      <c r="F54" s="11"/>
       <c r="G54" s="8"/>
       <c r="H54" s="8">
         <v>13.993237081</v>
       </c>
       <c r="I54" s="8" t="s">
-        <v>164</v>
-      </c>
-      <c r="J54" s="27"/>
+        <v>163</v>
+      </c>
+      <c r="J54" s="20"/>
     </row>
     <row r="55" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A55" s="9"/>
-      <c r="B55" s="18">
+      <c r="A55" s="26"/>
+      <c r="B55" s="22">
         <v>0.75</v>
       </c>
-      <c r="C55" s="22">
+      <c r="C55" s="15">
         <v>0.1</v>
       </c>
-      <c r="D55" s="21" t="s">
+      <c r="D55" s="14" t="s">
+        <v>168</v>
+      </c>
+      <c r="E55" s="9" t="s">
+        <v>167</v>
+      </c>
+      <c r="F55" s="12"/>
+      <c r="G55" s="9"/>
+      <c r="H55" s="9">
+        <v>6.9898355999999995E-2</v>
+      </c>
+      <c r="I55" s="9" t="s">
+        <v>166</v>
+      </c>
+      <c r="J55" s="17"/>
+    </row>
+    <row r="56" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A56" s="26"/>
+      <c r="B56" s="23"/>
+      <c r="C56" s="15">
+        <v>0.01</v>
+      </c>
+      <c r="D56" s="5" t="s">
+        <v>170</v>
+      </c>
+      <c r="E56" s="7" t="s">
         <v>169</v>
       </c>
-      <c r="E55" s="12" t="s">
-        <v>168</v>
-      </c>
-      <c r="F55" s="15"/>
-      <c r="G55" s="12"/>
-      <c r="H55" s="12">
-        <v>6.9898355999999995E-2</v>
-      </c>
-      <c r="I55" s="12" t="s">
-        <v>167</v>
-      </c>
-      <c r="J55" s="24"/>
-    </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A56" s="9"/>
-      <c r="B56" s="19"/>
-      <c r="C56" s="22">
-        <v>0.01</v>
-      </c>
-      <c r="D56" s="5" t="s">
-        <v>171</v>
-      </c>
-      <c r="E56" s="7" t="s">
-        <v>170</v>
-      </c>
-      <c r="F56" s="16"/>
+      <c r="F56" s="13"/>
       <c r="H56" s="7">
         <v>9.8977041000000002E-2</v>
       </c>
       <c r="I56" s="7" t="s">
-        <v>172</v>
-      </c>
-      <c r="J56" s="24"/>
+        <v>171</v>
+      </c>
+      <c r="J56" s="17"/>
     </row>
     <row r="57" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A57" s="9"/>
-      <c r="B57" s="19"/>
-      <c r="C57" s="22">
+      <c r="A57" s="26"/>
+      <c r="B57" s="23"/>
+      <c r="C57" s="15">
         <v>1E-3</v>
       </c>
       <c r="D57" s="5" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="E57" s="7" t="s">
-        <v>174</v>
-      </c>
-      <c r="F57" s="16"/>
+        <v>173</v>
+      </c>
+      <c r="F57" s="13"/>
       <c r="H57" s="7">
         <v>0.433358723</v>
       </c>
       <c r="I57" s="7" t="s">
-        <v>173</v>
-      </c>
-      <c r="J57" s="24"/>
+        <v>172</v>
+      </c>
+      <c r="J57" s="17"/>
     </row>
     <row r="58" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="9"/>
-      <c r="B58" s="20"/>
-      <c r="C58" s="23">
+      <c r="A58" s="26"/>
+      <c r="B58" s="24"/>
+      <c r="C58" s="16">
         <v>1E-4</v>
       </c>
       <c r="D58" s="6" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="E58" s="8" t="s">
-        <v>177</v>
-      </c>
-      <c r="F58" s="14"/>
+        <v>176</v>
+      </c>
+      <c r="F58" s="11"/>
       <c r="G58" s="8"/>
       <c r="H58" s="8">
         <v>2.7366274829999999</v>
       </c>
       <c r="I58" s="8" t="s">
-        <v>176</v>
-      </c>
-      <c r="J58" s="28"/>
+        <v>175</v>
+      </c>
+      <c r="J58" s="21"/>
     </row>
     <row r="59" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A59" s="9"/>
-      <c r="B59" s="19">
+      <c r="A59" s="26"/>
+      <c r="B59" s="23">
         <v>0.99</v>
       </c>
-      <c r="C59" s="22">
+      <c r="C59" s="15">
         <v>0.1</v>
       </c>
       <c r="D59" s="5" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="E59" s="7" t="s">
-        <v>179</v>
-      </c>
-      <c r="F59" s="16"/>
+        <v>178</v>
+      </c>
+      <c r="F59" s="13"/>
       <c r="H59" s="7">
         <v>6.5501029000000002E-2</v>
       </c>
       <c r="I59" s="7" t="s">
-        <v>181</v>
-      </c>
-      <c r="J59" s="24"/>
+        <v>180</v>
+      </c>
+      <c r="J59" s="17"/>
     </row>
     <row r="60" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A60" s="9"/>
-      <c r="B60" s="19"/>
-      <c r="C60" s="22">
+      <c r="A60" s="26"/>
+      <c r="B60" s="23"/>
+      <c r="C60" s="15">
         <v>0.01</v>
       </c>
       <c r="D60" s="5" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="E60" s="7" t="s">
-        <v>183</v>
-      </c>
-      <c r="F60" s="16"/>
+        <v>182</v>
+      </c>
+      <c r="F60" s="13"/>
       <c r="H60" s="7">
         <v>9.7620693999999994E-2</v>
       </c>
       <c r="I60" s="7" t="s">
-        <v>182</v>
-      </c>
-      <c r="J60" s="24"/>
+        <v>181</v>
+      </c>
+      <c r="J60" s="17"/>
     </row>
     <row r="61" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A61" s="9"/>
-      <c r="B61" s="19"/>
-      <c r="C61" s="22">
+      <c r="A61" s="26"/>
+      <c r="B61" s="23"/>
+      <c r="C61" s="15">
         <v>1E-3</v>
       </c>
       <c r="D61" s="5" t="s">
+        <v>185</v>
+      </c>
+      <c r="E61" s="7" t="s">
         <v>186</v>
       </c>
-      <c r="E61" s="7" t="s">
-        <v>187</v>
-      </c>
-      <c r="F61" s="16"/>
+      <c r="F61" s="13"/>
       <c r="H61" s="7">
         <v>0.34670059800000003</v>
       </c>
       <c r="I61" s="7" t="s">
-        <v>185</v>
-      </c>
-      <c r="J61" s="24"/>
+        <v>184</v>
+      </c>
+      <c r="J61" s="17"/>
     </row>
     <row r="62" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="10"/>
-      <c r="B62" s="20"/>
-      <c r="C62" s="23">
+      <c r="A62" s="27"/>
+      <c r="B62" s="24"/>
+      <c r="C62" s="16">
         <v>1E-4</v>
       </c>
       <c r="D62" s="6" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="E62" s="8" t="s">
-        <v>189</v>
-      </c>
-      <c r="F62" s="14"/>
+        <v>188</v>
+      </c>
+      <c r="F62" s="11"/>
       <c r="G62" s="8"/>
       <c r="H62" s="8">
         <v>2.7786704009999998</v>
       </c>
       <c r="I62" s="8" t="s">
-        <v>188</v>
-      </c>
-      <c r="J62" s="28"/>
+        <v>187</v>
+      </c>
+      <c r="J62" s="21"/>
     </row>
   </sheetData>
   <mergeCells count="19">
-    <mergeCell ref="B23:B26"/>
-    <mergeCell ref="B27:B30"/>
-    <mergeCell ref="B31:B34"/>
-    <mergeCell ref="B35:B38"/>
-    <mergeCell ref="B39:B42"/>
+    <mergeCell ref="A1:G1"/>
+    <mergeCell ref="A3:A22"/>
+    <mergeCell ref="B3:B6"/>
+    <mergeCell ref="B7:B10"/>
+    <mergeCell ref="B11:B14"/>
+    <mergeCell ref="B19:B22"/>
+    <mergeCell ref="B15:B18"/>
     <mergeCell ref="B43:B46"/>
     <mergeCell ref="B47:B50"/>
     <mergeCell ref="B51:B54"/>
@@ -2588,13 +2590,11 @@
     <mergeCell ref="A43:A62"/>
     <mergeCell ref="B55:B58"/>
     <mergeCell ref="B59:B62"/>
-    <mergeCell ref="A1:G1"/>
-    <mergeCell ref="A3:A22"/>
-    <mergeCell ref="B3:B6"/>
-    <mergeCell ref="B7:B10"/>
-    <mergeCell ref="B11:B14"/>
-    <mergeCell ref="B19:B22"/>
-    <mergeCell ref="B15:B18"/>
+    <mergeCell ref="B23:B26"/>
+    <mergeCell ref="B27:B30"/>
+    <mergeCell ref="B31:B34"/>
+    <mergeCell ref="B35:B38"/>
+    <mergeCell ref="B39:B42"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>